<commit_message>
Added try/catch. Expanded aliases
</commit_message>
<xml_diff>
--- a/Examples/CustomReporting/dashboard.xlsx
+++ b/Examples/CustomReporting/dashboard.xlsx
@@ -35,25 +35,25 @@
     <t>%</t>
   </si>
   <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
     <t>Phoneix</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Newark</t>
-  </si>
-  <si>
-    <t>Philadelphia</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
   </si>
   <si>
     <t>Grand Total Calculation</t>
@@ -163,9 +163,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.9776763916016" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="0.75" customWidth="1"/>
-    <col min="3" max="3" width="11.1730823516846" customWidth="1"/>
+    <col min="3" max="3" width="12.2299089431763" customWidth="1"/>
     <col min="4" max="4" width="0.75" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1" style="1"/>
     <col min="6" max="6" width="0.75" customWidth="1"/>
@@ -230,157 +230,157 @@
         <v>8</v>
       </c>
       <c r="E3" s="1">
-        <v>18075614</v>
+        <v>3602000</v>
       </c>
       <c r="G3" s="2">
-        <v>0.3276</v>
+        <v>0.0809</v>
       </c>
       <c r="I3" s="1">
-        <v>3434680</v>
+        <v>955000</v>
       </c>
       <c r="K3" s="2">
-        <v>0.39</v>
+        <v>0.09</v>
       </c>
       <c r="M3" s="3">
-        <v>588</v>
+        <v>245</v>
       </c>
       <c r="O3" s="3">
-        <v>-8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
-        <v>2403235</v>
+        <v>4674000</v>
       </c>
       <c r="G4" s="2">
-        <v>0.6968</v>
+        <v>0.105</v>
       </c>
       <c r="I4" s="1">
-        <v>68430</v>
+        <v>336000</v>
       </c>
       <c r="K4" s="2">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
       <c r="M4" s="3">
-        <v>961</v>
+        <v>222</v>
       </c>
       <c r="O4" s="3">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
-        <v>6748467</v>
+        <v>4674000</v>
       </c>
       <c r="G5" s="2">
-        <v>0.3166</v>
+        <v>0.0804</v>
       </c>
       <c r="I5" s="1">
-        <v>9460287</v>
+        <v>1536000</v>
       </c>
       <c r="K5" s="2">
-        <v>0.09</v>
+        <v>0.14</v>
       </c>
       <c r="M5" s="3">
-        <v>617</v>
+        <v>550</v>
       </c>
       <c r="O5" s="3">
-        <v>-50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1">
-        <v>10664444</v>
+        <v>12180000</v>
       </c>
       <c r="G6" s="2">
-        <v>0.1175</v>
+        <v>0.1427</v>
       </c>
       <c r="I6" s="1">
-        <v>5954576</v>
+        <v>-716000</v>
       </c>
       <c r="K6" s="2">
-        <v>-0.03</v>
+        <v>-0.07</v>
       </c>
       <c r="M6" s="3">
-        <v>632</v>
+        <v>321</v>
       </c>
       <c r="O6" s="3">
-        <v>14</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="1">
-        <v>85020237</v>
+        <v>3221000</v>
       </c>
       <c r="G7" s="2">
-        <v>0.8978</v>
+        <v>0.0629</v>
       </c>
       <c r="I7" s="1">
-        <v>1547582</v>
+        <v>1088000</v>
       </c>
       <c r="K7" s="2">
-        <v>-0.95</v>
+        <v>0.04</v>
       </c>
       <c r="M7" s="3">
-        <v>569</v>
+        <v>436</v>
       </c>
       <c r="O7" s="3">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1">
-        <v>65484315</v>
+        <v>2782000</v>
       </c>
       <c r="G8" s="2">
-        <v>0.3988</v>
+        <v>0.0723</v>
       </c>
       <c r="I8" s="1">
-        <v>2307078</v>
+        <v>467000</v>
       </c>
       <c r="K8" s="2">
-        <v>-0.45</v>
+        <v>0.1</v>
       </c>
       <c r="M8" s="3">
-        <v>221</v>
+        <v>674</v>
       </c>
       <c r="O8" s="3">
-        <v>-92</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">

</xml_diff>